<commit_message>
HFDA -ch3part2 Add constraints on sales_volume
</commit_message>
<xml_diff>
--- a/book6_headFirstDataAnalysis/bathing_friends_unlimited.xlsx
+++ b/book6_headFirstDataAnalysis/bathing_friends_unlimited.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\夏舒阳\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\github\base\book6_headFirstDataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,14 +23,16 @@
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$13</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$B$6</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$B$5</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$B$6</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$B$6</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$B$20</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
@@ -38,9 +40,13 @@
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$B$14</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">400</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">300</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">150</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">400</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">300</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">50</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -437,19 +443,19 @@
   <dimension ref="B5:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="5" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B5">
-        <v>400</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B6">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.15">
@@ -458,7 +464,7 @@
       </c>
       <c r="C10">
         <f>B10*B5</f>
-        <v>40000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.15">
@@ -467,13 +473,13 @@
       </c>
       <c r="C11">
         <f>B11*B6</f>
-        <v>10000</v>
+        <v>6250</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B13">
         <f>C10+C11</f>
-        <v>50000</v>
+        <v>21250</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.15">
@@ -494,7 +500,7 @@
     <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20">
         <f>B17*B5+B18*B6</f>
-        <v>2320</v>
+        <v>950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>